<commit_message>
order of CONVERTED PLASMA and RAILGUN accuracy
</commit_message>
<xml_diff>
--- a/WorkFiles/Shooting.xlsx
+++ b/WorkFiles/Shooting.xlsx
@@ -1396,8 +1396,8 @@
   </sheetPr>
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N27" activeCellId="0" sqref="N27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2368,7 +2368,7 @@
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="17" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>

</xml_diff>